<commit_message>
reform orders file + add opportunity to expand orders to see their items
</commit_message>
<xml_diff>
--- a/src/main/resources/database/order_items.xlsx
+++ b/src/main/resources/database/order_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\clothing-store\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4AC503-07EE-4EEC-8E9A-47B138BA15FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA4FC30-AA7F-4FDE-83DF-07190250EF0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+  <si>
+    <t>paid</t>
+  </si>
+  <si>
+    <t>booked</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,214 +349,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="C1" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="D1" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>102.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>102.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>102.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>110.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>129.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4.0</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>58</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>91</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>106.0</v>
+        <v>2.0</v>
       </c>
       <c r="B6" t="n">
-        <v>90.0</v>
+        <v>58.0</v>
       </c>
       <c r="C6" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="D6" t="n">
         <v>8.0</v>
       </c>
-      <c r="E6" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>106.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B11" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B13" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B14" t="n">
-        <v>58.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="17"/>
-    <row r="18"/>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>